<commit_message>
added and changed some games
</commit_message>
<xml_diff>
--- a/Docs/Missing Games (10 July 2025).xlsx
+++ b/Docs/Missing Games (10 July 2025).xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="568">
   <si>
     <t xml:space="preserve">GAME NAME</t>
   </si>
@@ -1152,6 +1152,12 @@
   </si>
   <si>
     <t xml:space="preserve">7f9fdad2f596ad4b8ace178aa588215b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radical Dreamers - Nusume Nai Houseki (Japan) (2-24) (En) (v1.4) (Demiforce) (MSU-1) (Cubear) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1489ae44423b19793dd6baf779b4884a </t>
   </si>
   <si>
     <t xml:space="preserve">nes/finalfaniii.7z &lt;Final Fantasy III (Japan)&gt;</t>
@@ -1738,7 +1744,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1800,6 +1806,13 @@
       <sz val="12"/>
       <name val="Consolas"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1889,7 +1902,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1970,6 +1983,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1978,7 +1995,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1990,19 +2007,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2010,11 +2027,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2216,7 +2233,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="1" sqref="D:D A4"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2292,20 +2309,20 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="D:D A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="51.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="70.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="24" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="51.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="70.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="25" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -2315,11 +2332,11 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>545</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>546</v>
+      <c r="A2" s="27" t="s">
+        <v>547</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>548</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>8</v>
@@ -2346,7 +2363,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="1" sqref="D:D A7"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2357,7 +2374,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="11" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="28" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="29" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2368,92 +2385,92 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" s="28" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="29" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>551</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="4" s="28" customFormat="true" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" s="29" customFormat="true" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="5" s="28" customFormat="true" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="5" s="29" customFormat="true" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>556</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4272,12 +4289,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C183"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
+      <selection pane="bottomLeft" activeCell="B183" activeCellId="0" sqref="B183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6287,6 +6304,17 @@
         <v>373</v>
       </c>
       <c r="C182" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="B183" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="C183" s="17" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6311,14 +6339,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="1" sqref="D:D A7"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="103.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="57.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="21" width="100.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="103.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="57.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="100.14"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6334,10 +6362,10 @@
     </row>
     <row r="2" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>8</v>
@@ -6345,21 +6373,21 @@
     </row>
     <row r="3" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>8</v>
@@ -6386,18 +6414,18 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="1" sqref="D:D B2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="64.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="48.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="70.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="24" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="64.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="48.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="70.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="25" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -6410,10 +6438,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>8</v>
@@ -6421,10 +6449,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>8</v>
@@ -6432,10 +6460,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>8</v>
@@ -6443,10 +6471,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>8</v>
@@ -6454,10 +6482,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>8</v>
@@ -6465,10 +6493,10 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>8</v>
@@ -6476,10 +6504,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>8</v>
@@ -6487,10 +6515,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>8</v>
@@ -6498,10 +6526,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>8</v>
@@ -6509,10 +6537,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>8</v>
@@ -6520,10 +6548,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>8</v>
@@ -6531,10 +6559,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>8</v>
@@ -6542,10 +6570,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>8</v>
@@ -6553,10 +6581,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>8</v>
@@ -6564,10 +6592,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>8</v>
@@ -6575,10 +6603,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>8</v>
@@ -6586,10 +6614,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>8</v>
@@ -6597,10 +6625,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>8</v>
@@ -6608,10 +6636,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>8</v>
@@ -6619,10 +6647,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>8</v>
@@ -6630,10 +6658,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>8</v>
@@ -6641,10 +6669,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>8</v>
@@ -6652,10 +6680,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>8</v>
@@ -6663,10 +6691,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>8</v>
@@ -6674,10 +6702,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>8</v>
@@ -6685,10 +6713,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>8</v>
@@ -6696,10 +6724,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>8</v>
@@ -6707,10 +6735,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>8</v>
@@ -6718,10 +6746,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>8</v>
@@ -6729,10 +6757,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>8</v>
@@ -6740,10 +6768,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>8</v>
@@ -6751,10 +6779,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>8</v>
@@ -6762,10 +6790,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>8</v>
@@ -6773,10 +6801,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>8</v>
@@ -6784,10 +6812,10 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>8</v>
@@ -6795,10 +6823,10 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>8</v>
@@ -6806,10 +6834,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>8</v>
@@ -6817,10 +6845,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>8</v>
@@ -6828,10 +6856,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C40" s="17" t="s">
         <v>8</v>
@@ -6839,10 +6867,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>8</v>
@@ -6850,10 +6878,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>8</v>
@@ -6861,10 +6889,10 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>8</v>
@@ -6872,10 +6900,10 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C44" s="17" t="s">
         <v>8</v>
@@ -6883,10 +6911,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>8</v>
@@ -6894,10 +6922,10 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>8</v>
@@ -6905,10 +6933,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>8</v>
@@ -6916,10 +6944,10 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>8</v>
@@ -6927,10 +6955,10 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>8</v>
@@ -6938,10 +6966,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C50" s="17" t="s">
         <v>8</v>
@@ -6949,10 +6977,10 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>8</v>
@@ -6960,10 +6988,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>8</v>
@@ -6990,20 +7018,20 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="D:D B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="75.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="43.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="70.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="24" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="75.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="43.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="70.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="25" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -7014,24 +7042,24 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>487</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -7053,20 +7081,20 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D:D B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="49.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="34.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="70.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="24" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="49.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="34.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="70.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="25" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -7076,11 +7104,11 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>488</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>489</v>
+      <c r="A2" s="27" t="s">
+        <v>490</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>491</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>8</v>
@@ -7107,20 +7135,20 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="1" sqref="D:D B2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="32.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="70.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="24" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="32.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="70.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="25" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -7130,11 +7158,11 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>490</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>491</v>
+      <c r="A2" s="27" t="s">
+        <v>492</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>493</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>8</v>
@@ -7161,17 +7189,17 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="D:D A3"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="112.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="47.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="98.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="112.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="47.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="21" width="98.86"/>
   </cols>
   <sheetData>
-    <row r="1" s="28" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="29" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -7184,288 +7212,288 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>497</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29" t="s">
-        <v>498</v>
+      <c r="A5" s="30" t="s">
+        <v>500</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="30" t="s">
         <v>500</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29" t="s">
-        <v>498</v>
-      </c>
       <c r="B6" s="9" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -7489,18 +7517,18 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="1" sqref="D:D A5"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="33.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="94.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="24" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="94.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="25" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7511,19 +7539,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>542</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>543</v>
-      </c>
-      <c r="C2" s="31" t="s">
+    <row r="2" s="28" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="27" t="s">
         <v>544</v>
       </c>
+      <c r="B2" s="31" t="s">
+        <v>545</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>546</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="32"/>
+      <c r="C3" s="33"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>